<commit_message>
export result to excel
</commit_message>
<xml_diff>
--- a/AutoTestProject/bin/Debug/TestCase.xlsx
+++ b/AutoTestProject/bin/Debug/TestCase.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Ten</t>
   </si>
@@ -35,9 +35,15 @@
     <t>LoiNhuan</t>
   </si>
   <si>
+    <t>Result</t>
+  </si>
+  <si>
     <t>Nhẫn 1</t>
   </si>
   <si>
+    <t>Chiếc</t>
+  </si>
+  <si>
     <t>Nhẫn2</t>
   </si>
   <si>
@@ -63,16 +69,14 @@
   </si>
   <si>
     <t>Nhẫn 10</t>
-  </si>
-  <si>
-    <t>Chiếc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,142 +386,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.77734375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0">
+        <v>2</v>
+      </c>
+      <c r="D3" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0">
+        <v>3</v>
+      </c>
+      <c r="D4" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0">
+        <v>4</v>
+      </c>
+      <c r="D5" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0">
+        <v>7</v>
+      </c>
+      <c r="D9" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="0">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="D10" s="0">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="0">
+        <v>7</v>
+      </c>
+      <c r="D11" s="0">
         <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>